<commit_message>
Atualizado lista de game
</commit_message>
<xml_diff>
--- a/Source/Terminal/Files/My game list.xlsx
+++ b/Source/Terminal/Files/My game list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2193a2b127f7beeb/Documents/My games/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{92574023-C763-47E4-8694-BC7782B2ED97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA2434DB-F76B-452A-8399-D1D01A11CC40}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{92574023-C763-47E4-8694-BC7782B2ED97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93C49B63-140C-4ACF-A1A0-E7C14E8F3053}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2955" yWindow="5265" windowWidth="22590" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="2925" windowWidth="20895" windowHeight="16785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="My game list" sheetId="1" r:id="rId1"/>
@@ -1098,12 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,6 +1154,9 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1172,8 +1174,11 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1189,8 +1194,11 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1206,8 +1214,11 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1243,6 +1254,9 @@
       <c r="E7" t="s">
         <v>13</v>
       </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1260,6 +1274,9 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1277,8 +1294,11 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1293,6 +1313,9 @@
       </c>
       <c r="E10" t="s">
         <v>17</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1311,6 +1334,9 @@
       <c r="E11" t="s">
         <v>7</v>
       </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1328,8 +1354,11 @@
       <c r="E12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1365,6 +1394,9 @@
       <c r="E14" t="s">
         <v>22</v>
       </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1382,6 +1414,9 @@
       <c r="E15" t="s">
         <v>7</v>
       </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1399,8 +1434,11 @@
       <c r="E16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1416,8 +1454,11 @@
       <c r="E17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1433,8 +1474,11 @@
       <c r="E18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1450,8 +1494,11 @@
       <c r="E19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1467,8 +1514,11 @@
       <c r="E20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1484,8 +1534,11 @@
       <c r="E21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1501,8 +1554,11 @@
       <c r="E22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1518,8 +1574,11 @@
       <c r="E23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1535,8 +1594,11 @@
       <c r="E24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1552,8 +1614,11 @@
       <c r="E25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1569,8 +1634,11 @@
       <c r="E26" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1586,8 +1654,11 @@
       <c r="E27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1603,8 +1674,11 @@
       <c r="E28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1620,8 +1694,11 @@
       <c r="E29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1637,8 +1714,11 @@
       <c r="E30" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1654,8 +1734,11 @@
       <c r="E31" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1670,6 +1753,9 @@
       </c>
       <c r="E32" t="s">
         <v>7</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,6 +1774,9 @@
       <c r="E33" t="s">
         <v>7</v>
       </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1705,6 +1794,9 @@
       <c r="E34" t="s">
         <v>7</v>
       </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1722,8 +1814,11 @@
       <c r="E35" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1739,8 +1834,11 @@
       <c r="E36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1756,8 +1854,11 @@
       <c r="E37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1773,8 +1874,11 @@
       <c r="E38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1789,6 +1893,9 @@
       </c>
       <c r="E39" t="s">
         <v>36</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1807,8 +1914,11 @@
       <c r="E40" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -1824,8 +1934,11 @@
       <c r="E41" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1840,6 +1953,9 @@
       </c>
       <c r="E42" t="s">
         <v>22</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1858,8 +1974,11 @@
       <c r="E43" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -1875,11 +1994,14 @@
       <c r="E44" t="s">
         <v>22</v>
       </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
       <c r="G44">
         <v>2014</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1895,11 +2017,14 @@
       <c r="E45" t="s">
         <v>22</v>
       </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
       <c r="G45">
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -1922,7 +2047,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1938,11 +2063,14 @@
       <c r="E47" t="s">
         <v>7</v>
       </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
       <c r="G47">
         <v>2017</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -1958,11 +2086,14 @@
       <c r="E48" t="s">
         <v>7</v>
       </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
       <c r="G48">
         <v>2014</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -1977,6 +2108,9 @@
       </c>
       <c r="E49" t="s">
         <v>22</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
       </c>
       <c r="G49">
         <v>2012</v>
@@ -1998,6 +2132,9 @@
       <c r="E50" t="s">
         <v>7</v>
       </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
       <c r="G50">
         <v>2016</v>
       </c>
@@ -2018,15 +2155,12 @@
       <c r="E51" t="s">
         <v>7</v>
       </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G51" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="FALSE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E43">
     <sortCondition ref="A2:A43"/>
   </sortState>

</xml_diff>